<commit_message>
Added technical replicates workflow and changed some functions according to this workflow
</commit_message>
<xml_diff>
--- a/Annotations_primers_template.xlsx
+++ b/Annotations_primers_template.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u0099120\Dropbox\Shared R projects\RT-qPCR\RT-qPCR\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="6510" yWindow="0" windowWidth="18540" windowHeight="11895"/>
+    <workbookView xWindow="6510" yWindow="0" windowWidth="18540" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,17 +19,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Target 1</t>
   </si>
   <si>
-    <t>gene</t>
-  </si>
-  <si>
-    <t>primer</t>
-  </si>
-  <si>
     <t>Target 2</t>
   </si>
   <si>
@@ -80,13 +69,22 @@
     <t>Target 16</t>
   </si>
   <si>
-    <t>hkg</t>
+    <t>Gene</t>
+  </si>
+  <si>
+    <t>Primer</t>
+  </si>
+  <si>
+    <t>HKG</t>
+  </si>
+  <si>
+    <t>TRUE OR FALSE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -121,7 +119,7 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -391,7 +389,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -402,7 +400,7 @@
   <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -413,10 +411,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="C1" t="s">
         <v>18</v>
@@ -426,95 +424,98 @@
       <c r="A2" t="s">
         <v>0</v>
       </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
       <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D5" s="1"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D17" s="1"/>
     </row>

</xml_diff>